<commit_message>
LDF commit for change the call_mso's send type
(cherry picked from commit ae2789a831101f46c85701418c8ec676b7105747)
Signed-off-by: hytera170726574 <40571004+hytera170726574@users.noreply.github.com>
(cherry picked from commit 79c7128be54b02e46ce4e471c0571aaeb7b94e0f)
Signed-off-by: hytera170726574 <40571004+hytera170726574@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -50,323 +50,323 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>cpriotity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ccancel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>csec_monitor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cdis_connect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cbroadcast</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mail_list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tool_box</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>search_bar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>resource_tree_top</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>resource_tree_bottom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>310-172</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>344-185</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>366-185</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>530-168</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>335-212</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>366-212</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>395-212</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>454-212</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>485-212</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>336-226</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>514-256</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>339-294</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>416-294</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>494-294</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>422-212</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lstate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>319-203</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lstate1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>209-108</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>69-108</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0-250</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0-855</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>38-148</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cnumber</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgna_add</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>93-794</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgna_delete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>256-794</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgna_pannel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgna_o</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgna_c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>262-755</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>127-755</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>127-1055</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgna_alies</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>771-520</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgna_confirm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>846-581</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgna_cancel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>683-581</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>279-127</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgna_input_right</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1620-1079</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dgna_input_left</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cross_pannel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>122-660</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cross_delete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>223-660</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cross_add</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>262-622</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cross_o</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>127-922</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cross_c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>127-622</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cross_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>911-441</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cross_save</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1045-695</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cross_cancel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>873-695</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cross_disable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>252-660</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cross_delete_ok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1043-596</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cross_delete_cancel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>875-596</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>515-222</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cfull_duplex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>cemergency</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cfull_duplex</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cpriotity</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ccancel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>csec_monitor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cdis_connect</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cset</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cbroadcast</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mail_list</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tool_box</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>search_bar</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>resource_tree_top</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>resource_tree_bottom</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>310-172</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>344-185</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>366-185</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>530-168</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>335-212</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>366-212</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>395-212</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>454-212</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>485-212</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>336-226</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>514-256</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>339-294</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>416-294</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>494-294</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>422-212</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lstate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>319-203</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lstate1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>209-108</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>69-108</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0-250</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0-855</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>38-148</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cnumber</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgna_add</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>93-794</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgna_delete</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>256-794</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgna_pannel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgna_o</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgna_c</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>262-755</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>127-755</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>127-1055</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgna_alies</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>771-520</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgna_confirm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>846-581</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgna_cancel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>683-581</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>279-127</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgna_input_right</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1620-1079</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dgna_input_left</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cross_pannel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>122-660</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cross_delete</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>223-660</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cross_add</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>262-622</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cross_o</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>127-922</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cross_c</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>127-622</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cross_num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>911-441</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cross_save</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1045-695</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cross_cancel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>873-695</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cross_disable</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>252-660</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cross_delete_ok</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1043-596</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cross_delete_cancel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>875-596</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>515-222</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -717,7 +717,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -730,7 +730,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -744,7 +744,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -758,47 +758,47 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>87</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>86</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
@@ -806,15 +806,15 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
@@ -822,7 +822,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
@@ -830,47 +830,47 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -895,210 +895,210 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>